<commit_message>
service: creation api: party refactored
</commit_message>
<xml_diff>
--- a/project_plans/files/adatadbazis_struktura.xlsx
+++ b/project_plans/files/adatadbazis_struktura.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>creation_service</t>
   </si>
@@ -82,16 +82,46 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>email</t>
+  </si>
+  <si>
     <t>participants_ids</t>
   </si>
   <si>
     <t>foregin_key_list</t>
   </si>
   <si>
+    <t>valszeg: "123,432,132" fromaban</t>
+  </si>
+  <si>
     <t>quantity</t>
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>organizer_ids</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>valszeg: "123,432,132" fromaban</t>
+    </r>
+  </si>
+  <si>
+    <t>participant_ids</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>valszeg: "123,432,132" fromaban</t>
+    </r>
   </si>
   <si>
     <t>drink_requirement</t>
@@ -215,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -248,6 +278,9 @@
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -590,28 +623,55 @@
       <c r="H6" s="14" t="s">
         <v>22</v>
       </c>
+      <c r="I6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="L6" s="11"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="11"/>
+      <c r="K7" s="15" t="s">
+        <v>30</v>
+      </c>
       <c r="L7" s="11"/>
     </row>
     <row r="8">
       <c r="D8" s="11"/>
       <c r="H8" s="11"/>
+      <c r="I8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>32</v>
+      </c>
       <c r="L8" s="11"/>
     </row>
     <row r="9">
@@ -630,32 +690,32 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
     </row>
     <row r="13">
       <c r="D13" s="11"/>
@@ -669,11 +729,11 @@
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H15" s="9"/>
       <c r="L15" s="11"/>
@@ -731,10 +791,10 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="10" t="s">
@@ -744,7 +804,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>22</v>
@@ -753,17 +813,17 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H20" s="11"/>
       <c r="L20" s="11"/>
@@ -785,7 +845,7 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D24" s="9"/>
       <c r="H24" s="11"/>
@@ -826,10 +886,10 @@
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D28" s="11"/>
       <c r="H28" s="11"/>
@@ -837,7 +897,7 @@
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
service: creation api: drinkRequirements implemented 1/1
</commit_message>
<xml_diff>
--- a/project_plans/files/adatadbazis_struktura.xlsx
+++ b/project_plans/files/adatadbazis_struktura.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>creation_service</t>
   </si>
@@ -112,6 +112,9 @@
     </r>
   </si>
   <si>
+    <t>desctiption</t>
+  </si>
+  <si>
     <t>participant_ids</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
   </si>
   <si>
     <t>quantity_mark</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
   <si>
     <t>food_requirement</t>
@@ -662,15 +668,21 @@
     </row>
     <row r="8">
       <c r="D8" s="11"/>
+      <c r="E8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="H8" s="11"/>
       <c r="I8" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L8" s="11"/>
     </row>
@@ -729,11 +741,11 @@
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H15" s="9"/>
       <c r="L15" s="11"/>
@@ -791,7 +803,7 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>28</v>
@@ -804,7 +816,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>22</v>
@@ -813,7 +825,7 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>9</v>
@@ -830,6 +842,12 @@
     </row>
     <row r="21">
       <c r="D21" s="11"/>
+      <c r="E21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="H21" s="11"/>
       <c r="L21" s="11"/>
     </row>
@@ -845,7 +863,7 @@
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D24" s="9"/>
       <c r="H24" s="11"/>
@@ -886,7 +904,7 @@
     </row>
     <row r="28">
       <c r="A28" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>28</v>
@@ -897,7 +915,7 @@
     </row>
     <row r="29">
       <c r="A29" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>9</v>

</xml_diff>